<commit_message>
Convert charts to altair
</commit_message>
<xml_diff>
--- a/aggregated_electricity.xlsx
+++ b/aggregated_electricity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\notes\PycharmProjects\optigram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAC0D11-E0E4-4150-9B2A-D8564B31CEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDBB404-6C8D-4B1B-971A-F4AE342AC3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="0" windowWidth="20640" windowHeight="16680" xr2:uid="{8C48A84A-50CE-4ECF-99EC-C96681CDE2C1}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{8C48A84A-50CE-4ECF-99EC-C96681CDE2C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,10 +54,10 @@
     <t>Landed Properties</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Usage</t>
+  </si>
+  <si>
+    <t>Housing</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,10 +455,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>